<commit_message>
the testing stage of the backend has been completed
</commit_message>
<xml_diff>
--- a/заполнение бд/shopCart.xlsx
+++ b/заполнение бд/shopCart.xlsx
@@ -360,7 +360,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -384,21 +384,21 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
         <v>3</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>